<commit_message>
Chaned ndt matching method parameter in TA template
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6705E02C-6374-4361-82AD-E2B1F98DDAD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949D2C39-2E53-40FC-8E21-1CC12419FF05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10470" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,21 +1138,21 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35:G48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="1" customWidth="1"/>
-    <col min="7" max="7" width="134.7109375" customWidth="1"/>
+    <col min="7" max="7" width="134.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1482,10 +1482,10 @@
         <v>3</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>224</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>224</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>224</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>224</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>224</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>224</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>224</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>224</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>224</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>23</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>23</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>23</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>23</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>-0.37059999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>-0.62939999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>23</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>23</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>23</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>23</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>23</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>23</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>23</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>23</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>23</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>23</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>23</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>23</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>23</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>23</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>23</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>23</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>23</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>23</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>23</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>23</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>23</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>23</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>23</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>23</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>23</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>23</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>23</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>23</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>23</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>23</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>23</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>23</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>23</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>23</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>23</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>23</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>23</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>23</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>23</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>23</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>23</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>23</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>23</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>23</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>23</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>23</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>23</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>23</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>23</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>23</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>23</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>23</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>23</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>23</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>23</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>23</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>23</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>23</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>23</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>23</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>23</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>23</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>23</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>23</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>23</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>23</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>23</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>23</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>23</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>23</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>23</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>23</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>23</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>23</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>23</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>23</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>23</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>23</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>23</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>23</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>23</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>23</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>23</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>23</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>23</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>23</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>23</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>23</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>23</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>23</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>23</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>23</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>23</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>23</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>23</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>23</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>23</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>23</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>23</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>23</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>23</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>23</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>23</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>23</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>23</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>23</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>23</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>23</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>23</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>23</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>23</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>23</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>23</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>23</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>23</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>23</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>23</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>23</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>23</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>23</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>23</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>23</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>23</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>23</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>23</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>23</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>23</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>23</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>23</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>213</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>213</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>213</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>213</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>213</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>213</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>213</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>213</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>213</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>214</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>214</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>214</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>214</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>214</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>214</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>214</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>214</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>214</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>214</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>214</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>214</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>214</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>214</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>214</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>214</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>214</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>214</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>214</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>214</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>214</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>214</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>214</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>214</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>214</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>214</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>214</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>214</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>214</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>214</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>214</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>214</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>214</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>214</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>214</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>214</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>214</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>214</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>214</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>214</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>214</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>214</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>214</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>214</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>226</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>228</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
Fixed test automation parameters for Experiment A of the lidar rain experiments
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949D2C39-2E53-40FC-8E21-1CC12419FF05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAE553C-EA81-4856-ACC7-2682A7E14B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="C179" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G195" sqref="G195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4172,7 +4172,7 @@
       </c>
       <c r="F143" s="5"/>
       <c r="G143" s="5">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -4296,7 +4296,7 @@
         <v>10</v>
       </c>
       <c r="G149" s="5">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -5207,7 +5207,7 @@
         <v>20</v>
       </c>
       <c r="G194" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -5230,7 +5230,7 @@
         <v>50</v>
       </c>
       <c r="G195" s="5">
-        <v>11.1</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -5322,7 +5322,7 @@
         <v>100</v>
       </c>
       <c r="G199" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -5601,7 +5601,7 @@
         <v>10</v>
       </c>
       <c r="G212" s="5">
-        <v>1.85</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -5624,7 +5624,7 @@
         <v>10</v>
       </c>
       <c r="G213" s="5">
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -5647,7 +5647,7 @@
         <v>10</v>
       </c>
       <c r="G214" s="5">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added workaround for PreScan TA issue with federates
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAE553C-EA81-4856-ACC7-2682A7E14B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C9C839-950E-4556-9E8A-F143BEB6E9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15996" yWindow="1272" windowWidth="14724" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C179" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G195" sqref="G195"/>
+    <sheetView tabSelected="1" topLeftCell="G134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4172,7 +4172,7 @@
       </c>
       <c r="F143" s="5"/>
       <c r="G143" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated TA template parameters
Removed the parameters that were unused for the imm_ukf node (they had no effect).
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE4764D-408F-48AB-BF37-EB5552932153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682B2F65-7FFC-4077-9F4B-D4A1EC4859BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6744" yWindow="1596" windowWidth="14724" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="261">
   <si>
     <t>tf_x</t>
   </si>
@@ -751,9 +751,6 @@
     <t>BaseLink_to_camera1</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>BaseLink_to_camera2</t>
   </si>
   <si>
@@ -778,9 +775,6 @@
     <t>/map</t>
   </si>
   <si>
-    <t>/detection/object_tracker/</t>
-  </si>
-  <si>
     <t>detection_probability</t>
   </si>
   <si>
@@ -815,12 +809,6 @@
   </si>
   <si>
     <t>lane_frame</t>
-  </si>
-  <si>
-    <t>merge_distance_threshold</t>
-  </si>
-  <si>
-    <t>namespace</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1206,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G270"/>
+  <dimension ref="A1:G268"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B165" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D187" sqref="D187"/>
+      <selection activeCell="D200" sqref="D200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,7 +2118,7 @@
         <v>23</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>0</v>
@@ -2153,7 +2141,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>1</v>
@@ -2176,7 +2164,7 @@
         <v>23</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>2</v>
@@ -2199,7 +2187,7 @@
         <v>23</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>69</v>
@@ -2222,7 +2210,7 @@
         <v>23</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>70</v>
@@ -2245,7 +2233,7 @@
         <v>23</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>71</v>
@@ -2268,7 +2256,7 @@
         <v>23</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>72</v>
@@ -5055,10 +5043,10 @@
         <v>23</v>
       </c>
       <c r="B181" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C181" s="13" t="s">
         <v>243</v>
-      </c>
-      <c r="C181" s="13" t="s">
-        <v>244</v>
       </c>
       <c r="D181" s="5" t="s">
         <v>5</v>
@@ -5074,10 +5062,10 @@
         <v>23</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C182" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D182" s="5" t="s">
         <v>5</v>
@@ -5093,10 +5081,10 @@
         <v>23</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D183" s="5" t="s">
         <v>5</v>
@@ -5112,10 +5100,10 @@
         <v>23</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C184" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D184" s="5" t="s">
         <v>5</v>
@@ -5131,10 +5119,10 @@
         <v>23</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D185" s="5" t="s">
         <v>5</v>
@@ -5150,10 +5138,10 @@
         <v>23</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D186" s="5" t="s">
         <v>5</v>
@@ -5169,10 +5157,10 @@
         <v>23</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C187" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D187" s="5" t="s">
         <v>5</v>
@@ -5188,10 +5176,10 @@
         <v>23</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D188" s="5" t="s">
         <v>5</v>
@@ -5207,10 +5195,10 @@
         <v>23</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>5</v>
@@ -5226,10 +5214,10 @@
         <v>23</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C190" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D190" s="5" t="s">
         <v>19</v>
@@ -5237,7 +5225,7 @@
       <c r="E190" s="12"/>
       <c r="F190" s="12"/>
       <c r="G190" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -5245,10 +5233,10 @@
         <v>23</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>19</v>
@@ -5264,10 +5252,10 @@
         <v>23</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>19</v>
@@ -5275,7 +5263,7 @@
       <c r="E192" s="12"/>
       <c r="F192" s="12"/>
       <c r="G192" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -5283,10 +5271,10 @@
         <v>23</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D193" s="12" t="s">
         <v>63</v>
@@ -5302,10 +5290,10 @@
         <v>23</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>19</v>
@@ -5313,7 +5301,7 @@
       <c r="E194" s="12"/>
       <c r="F194" s="12"/>
       <c r="G194" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -5321,10 +5309,10 @@
         <v>23</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D195" s="5" t="s">
         <v>19</v>
@@ -5332,45 +5320,45 @@
       <c r="E195" s="5"/>
       <c r="F195" s="5"/>
       <c r="G195" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B196" s="12" t="s">
-        <v>243</v>
+      <c r="B196" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>263</v>
+        <v>120</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E196" s="5"/>
       <c r="F196" s="5"/>
-      <c r="G196" s="5" t="s">
-        <v>241</v>
+      <c r="G196" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B197" s="12" t="s">
-        <v>243</v>
+      <c r="B197" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>264</v>
+        <v>121</v>
       </c>
       <c r="D197" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E197" s="5"/>
       <c r="F197" s="5"/>
-      <c r="G197" s="5" t="s">
-        <v>250</v>
+      <c r="G197" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -5381,7 +5369,7 @@
         <v>119</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="D198" s="5" t="s">
         <v>19</v>
@@ -5389,7 +5377,7 @@
       <c r="E198" s="5"/>
       <c r="F198" s="5"/>
       <c r="G198" s="9" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -5400,15 +5388,15 @@
         <v>119</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D199" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E199" s="5"/>
       <c r="F199" s="5"/>
-      <c r="G199" s="9" t="s">
-        <v>128</v>
+      <c r="G199" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -5419,15 +5407,15 @@
         <v>119</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="D200" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
-      <c r="G200" s="9" t="s">
-        <v>84</v>
+      <c r="G200" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -5438,7 +5426,7 @@
         <v>119</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D201" s="5" t="s">
         <v>19</v>
@@ -5446,7 +5434,7 @@
       <c r="E201" s="5"/>
       <c r="F201" s="5"/>
       <c r="G201" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -5457,15 +5445,15 @@
         <v>119</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E202" s="5"/>
       <c r="F202" s="5"/>
-      <c r="G202" s="5" t="s">
-        <v>130</v>
+      <c r="G202" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -5476,15 +5464,19 @@
         <v>119</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D203" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E203" s="5"/>
-      <c r="F203" s="5"/>
-      <c r="G203" s="5" t="s">
-        <v>131</v>
+        <v>5</v>
+      </c>
+      <c r="E203" s="5">
+        <v>0</v>
+      </c>
+      <c r="F203" s="5">
+        <v>10</v>
+      </c>
+      <c r="G203" s="5">
+        <v>0.4</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -5492,18 +5484,18 @@
         <v>23</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E204" s="5"/>
       <c r="F204" s="5"/>
-      <c r="G204" s="5" t="b">
-        <v>0</v>
+      <c r="G204" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -5511,22 +5503,18 @@
         <v>23</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E205" s="5">
-        <v>0</v>
-      </c>
-      <c r="F205" s="5">
-        <v>10</v>
-      </c>
-      <c r="G205" s="5">
-        <v>0.4</v>
+        <v>19</v>
+      </c>
+      <c r="E205" s="5"/>
+      <c r="F205" s="5"/>
+      <c r="G205" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -5537,15 +5525,15 @@
         <v>132</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E206" s="5"/>
       <c r="F206" s="5"/>
-      <c r="G206" s="9" t="s">
-        <v>134</v>
+      <c r="G206" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -5553,10 +5541,10 @@
         <v>23</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D207" s="5" t="s">
         <v>19</v>
@@ -5564,7 +5552,7 @@
       <c r="E207" s="5"/>
       <c r="F207" s="5"/>
       <c r="G207" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -5572,18 +5560,18 @@
         <v>23</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D208" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E208" s="5"/>
       <c r="F208" s="5"/>
-      <c r="G208" s="5" t="b">
-        <v>0</v>
+      <c r="G208" s="9" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -5594,7 +5582,7 @@
         <v>135</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="D209" s="5" t="s">
         <v>19</v>
@@ -5602,7 +5590,7 @@
       <c r="E209" s="5"/>
       <c r="F209" s="5"/>
       <c r="G209" s="9" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -5613,7 +5601,7 @@
         <v>135</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="D210" s="5" t="s">
         <v>19</v>
@@ -5621,7 +5609,7 @@
       <c r="E210" s="5"/>
       <c r="F210" s="5"/>
       <c r="G210" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -5632,7 +5620,7 @@
         <v>135</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D211" s="5" t="s">
         <v>19</v>
@@ -5640,45 +5628,49 @@
       <c r="E211" s="5"/>
       <c r="F211" s="5"/>
       <c r="G211" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>23</v>
+        <v>213</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>137</v>
+        <v>24</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E212" s="5"/>
-      <c r="F212" s="5"/>
-      <c r="G212" s="9" t="s">
-        <v>141</v>
+        <v>5</v>
+      </c>
+      <c r="E212" s="5">
+        <v>0</v>
+      </c>
+      <c r="F212" s="5">
+        <v>2</v>
+      </c>
+      <c r="G212" s="5">
+        <v>0.75</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
-        <v>23</v>
+        <v>213</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>138</v>
+        <v>25</v>
       </c>
       <c r="D213" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E213" s="5"/>
       <c r="F213" s="5"/>
-      <c r="G213" s="9" t="s">
-        <v>142</v>
+      <c r="G213" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -5689,19 +5681,15 @@
         <v>212</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D214" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E214" s="5">
-        <v>0</v>
-      </c>
-      <c r="F214" s="5">
-        <v>2</v>
-      </c>
-      <c r="G214" s="5">
-        <v>0.75</v>
+        <v>63</v>
+      </c>
+      <c r="E214" s="5"/>
+      <c r="F214" s="5"/>
+      <c r="G214" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -5712,7 +5700,7 @@
         <v>212</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D215" s="5" t="s">
         <v>63</v>
@@ -5731,7 +5719,7 @@
         <v>212</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D216" s="5" t="s">
         <v>63</v>
@@ -5750,14 +5738,18 @@
         <v>212</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D217" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E217" s="5"/>
-      <c r="F217" s="5"/>
-      <c r="G217" s="5" t="b">
+        <v>20</v>
+      </c>
+      <c r="E217" s="5">
+        <v>0</v>
+      </c>
+      <c r="F217" s="5">
+        <v>2</v>
+      </c>
+      <c r="G217" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5769,14 +5761,18 @@
         <v>212</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D218" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E218" s="5"/>
-      <c r="F218" s="5"/>
-      <c r="G218" s="5" t="b">
+        <v>20</v>
+      </c>
+      <c r="E218" s="5">
+        <v>0</v>
+      </c>
+      <c r="F218" s="5">
+        <v>2</v>
+      </c>
+      <c r="G218" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5788,19 +5784,15 @@
         <v>212</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D219" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E219" s="5">
-        <v>0</v>
-      </c>
-      <c r="F219" s="5">
-        <v>2</v>
-      </c>
-      <c r="G219" s="5">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="E219" s="5"/>
+      <c r="F219" s="5"/>
+      <c r="G219" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -5811,49 +5803,53 @@
         <v>212</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="D220" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E220" s="5">
         <v>0</v>
       </c>
       <c r="F220" s="5">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G220" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>212</v>
+        <v>65</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D221" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E221" s="5"/>
-      <c r="F221" s="5"/>
-      <c r="G221" s="5" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E221" s="5">
+        <v>0</v>
+      </c>
+      <c r="F221" s="5">
+        <v>10</v>
+      </c>
+      <c r="G221" s="5">
+        <v>0.75</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>212</v>
+        <v>65</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>236</v>
+        <v>32</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>5</v>
@@ -5862,10 +5858,10 @@
         <v>0</v>
       </c>
       <c r="F222" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G222" s="5">
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -5876,7 +5872,7 @@
         <v>65</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D223" s="5" t="s">
         <v>5</v>
@@ -5885,10 +5881,10 @@
         <v>0</v>
       </c>
       <c r="F223" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G223" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -5899,7 +5895,7 @@
         <v>65</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D224" s="5" t="s">
         <v>5</v>
@@ -5908,10 +5904,10 @@
         <v>0</v>
       </c>
       <c r="F224" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G224" s="5">
-        <v>0.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -5922,7 +5918,7 @@
         <v>65</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D225" s="5" t="s">
         <v>5</v>
@@ -5931,10 +5927,10 @@
         <v>0</v>
       </c>
       <c r="F225" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G225" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -5945,7 +5941,7 @@
         <v>65</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D226" s="5" t="s">
         <v>5</v>
@@ -5954,10 +5950,10 @@
         <v>0</v>
       </c>
       <c r="F226" s="5">
+        <v>200</v>
+      </c>
+      <c r="G226" s="5">
         <v>50</v>
-      </c>
-      <c r="G226" s="5">
-        <v>5.5</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -5968,7 +5964,7 @@
         <v>65</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>5</v>
@@ -5977,10 +5973,10 @@
         <v>0</v>
       </c>
       <c r="F227" s="5">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="G227" s="5">
-        <v>0.1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -5991,7 +5987,7 @@
         <v>65</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>5</v>
@@ -6000,7 +5996,7 @@
         <v>0</v>
       </c>
       <c r="F228" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G228" s="5">
         <v>50</v>
@@ -6014,7 +6010,7 @@
         <v>65</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>5</v>
@@ -6023,10 +6019,10 @@
         <v>0</v>
       </c>
       <c r="F229" s="5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="G229" s="5">
-        <v>200</v>
+        <v>15</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -6037,7 +6033,7 @@
         <v>65</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>5</v>
@@ -6049,7 +6045,7 @@
         <v>100</v>
       </c>
       <c r="G230" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -6060,7 +6056,7 @@
         <v>65</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D231" s="5" t="s">
         <v>5</v>
@@ -6069,10 +6065,10 @@
         <v>0</v>
       </c>
       <c r="F231" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G231" s="5">
-        <v>15</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -6083,7 +6079,7 @@
         <v>65</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>5</v>
@@ -6092,10 +6088,10 @@
         <v>0</v>
       </c>
       <c r="F232" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G232" s="5">
-        <v>5</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -6106,7 +6102,7 @@
         <v>65</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D233" s="5" t="s">
         <v>5</v>
@@ -6118,7 +6114,7 @@
         <v>10</v>
       </c>
       <c r="G233" s="5">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -6129,7 +6125,7 @@
         <v>65</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D234" s="5" t="s">
         <v>5</v>
@@ -6141,7 +6137,7 @@
         <v>10</v>
       </c>
       <c r="G234" s="5">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -6152,7 +6148,7 @@
         <v>65</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D235" s="5" t="s">
         <v>5</v>
@@ -6164,7 +6160,7 @@
         <v>10</v>
       </c>
       <c r="G235" s="5">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -6175,19 +6171,15 @@
         <v>65</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D236" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E236" s="5">
-        <v>0</v>
-      </c>
-      <c r="F236" s="5">
-        <v>10</v>
-      </c>
-      <c r="G236" s="5">
-        <v>0.1</v>
+        <v>63</v>
+      </c>
+      <c r="E236" s="5"/>
+      <c r="F236" s="5"/>
+      <c r="G236" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -6198,19 +6190,15 @@
         <v>65</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D237" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E237" s="5">
-        <v>0</v>
-      </c>
-      <c r="F237" s="5">
-        <v>10</v>
-      </c>
-      <c r="G237" s="5">
-        <v>0.1</v>
+        <v>63</v>
+      </c>
+      <c r="E237" s="5"/>
+      <c r="F237" s="5"/>
+      <c r="G237" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -6221,7 +6209,7 @@
         <v>65</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D238" s="5" t="s">
         <v>63</v>
@@ -6240,7 +6228,7 @@
         <v>65</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D239" s="5" t="s">
         <v>63</v>
@@ -6248,7 +6236,7 @@
       <c r="E239" s="5"/>
       <c r="F239" s="5"/>
       <c r="G239" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -6259,7 +6247,7 @@
         <v>65</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D240" s="5" t="s">
         <v>63</v>
@@ -6278,15 +6266,19 @@
         <v>65</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E241" s="5"/>
-      <c r="F241" s="5"/>
-      <c r="G241" s="5" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E241" s="5">
+        <v>0</v>
+      </c>
+      <c r="F241" s="5">
+        <v>10</v>
+      </c>
+      <c r="G241" s="5">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -6297,15 +6289,19 @@
         <v>65</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D242" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E242" s="5"/>
-      <c r="F242" s="5"/>
-      <c r="G242" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E242" s="5">
+        <v>0</v>
+      </c>
+      <c r="F242" s="5">
+        <v>10</v>
+      </c>
+      <c r="G242" s="5">
+        <v>4.8</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -6316,7 +6312,7 @@
         <v>65</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D243" s="5" t="s">
         <v>5</v>
@@ -6328,7 +6324,7 @@
         <v>10</v>
       </c>
       <c r="G243" s="5">
-        <v>2.2000000000000002</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -6339,7 +6335,7 @@
         <v>65</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D244" s="5" t="s">
         <v>5</v>
@@ -6351,7 +6347,7 @@
         <v>10</v>
       </c>
       <c r="G244" s="5">
-        <v>4.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -6362,7 +6358,7 @@
         <v>65</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D245" s="5" t="s">
         <v>5</v>
@@ -6374,7 +6370,7 @@
         <v>10</v>
       </c>
       <c r="G245" s="5">
-        <v>2.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -6385,7 +6381,7 @@
         <v>65</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D246" s="5" t="s">
         <v>5</v>
@@ -6397,7 +6393,7 @@
         <v>10</v>
       </c>
       <c r="G246" s="5">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -6408,7 +6404,7 @@
         <v>65</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D247" s="5" t="s">
         <v>5</v>
@@ -6420,7 +6416,7 @@
         <v>10</v>
       </c>
       <c r="G247" s="5">
-        <v>0.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -6431,7 +6427,7 @@
         <v>65</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D248" s="5" t="s">
         <v>5</v>
@@ -6443,7 +6439,7 @@
         <v>10</v>
       </c>
       <c r="G248" s="5">
-        <v>1.2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -6454,19 +6450,19 @@
         <v>65</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D249" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E249" s="5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F249" s="5">
         <v>10</v>
       </c>
       <c r="G249" s="5">
-        <v>3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -6477,7 +6473,7 @@
         <v>65</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D250" s="5" t="s">
         <v>5</v>
@@ -6489,7 +6485,7 @@
         <v>10</v>
       </c>
       <c r="G250" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -6500,7 +6496,7 @@
         <v>65</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D251" s="5" t="s">
         <v>5</v>
@@ -6509,10 +6505,10 @@
         <v>-10</v>
       </c>
       <c r="F251" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G251" s="5">
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -6523,19 +6519,19 @@
         <v>65</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="D252" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E252" s="5">
         <v>0</v>
       </c>
       <c r="F252" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G252" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -6543,22 +6539,18 @@
         <v>214</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D253" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E253" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F253" s="5">
-        <v>0</v>
-      </c>
-      <c r="G253" s="5">
-        <v>-3</v>
+        <v>63</v>
+      </c>
+      <c r="E253" s="5"/>
+      <c r="F253" s="5"/>
+      <c r="G253" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -6566,21 +6558,17 @@
         <v>214</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E254" s="5">
-        <v>0</v>
-      </c>
-      <c r="F254" s="5">
-        <v>2</v>
-      </c>
-      <c r="G254" s="5">
+        <v>63</v>
+      </c>
+      <c r="E254" s="5"/>
+      <c r="F254" s="5"/>
+      <c r="G254" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6589,10 +6577,10 @@
         <v>214</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="D255" s="5" t="s">
         <v>63</v>
@@ -6608,18 +6596,22 @@
         <v>214</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E256" s="5"/>
-      <c r="F256" s="5"/>
-      <c r="G256" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E256" s="5">
+        <v>0</v>
+      </c>
+      <c r="F256" s="5">
+        <v>10</v>
+      </c>
+      <c r="G256" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -6630,26 +6622,30 @@
         <v>143</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E257" s="5"/>
-      <c r="F257" s="5"/>
-      <c r="G257" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E257" s="5">
+        <v>0</v>
+      </c>
+      <c r="F257" s="5">
+        <v>10</v>
+      </c>
+      <c r="G257" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B258" s="2" t="s">
-        <v>143</v>
+      <c r="B258" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D258" s="5" t="s">
         <v>5</v>
@@ -6658,10 +6654,10 @@
         <v>0</v>
       </c>
       <c r="F258" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G258" s="5">
-        <v>0.1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -6669,33 +6665,33 @@
         <v>214</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="D259" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E259" s="5">
         <v>0</v>
       </c>
       <c r="F259" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G259" s="5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B260" s="4" t="s">
-        <v>145</v>
+      <c r="B260" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D260" s="5" t="s">
         <v>5</v>
@@ -6707,7 +6703,7 @@
         <v>100</v>
       </c>
       <c r="G260" s="5">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -6718,19 +6714,19 @@
         <v>211</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E261" s="5">
         <v>0</v>
       </c>
       <c r="F261" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G261" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -6741,7 +6737,7 @@
         <v>211</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D262" s="5" t="s">
         <v>5</v>
@@ -6750,10 +6746,10 @@
         <v>0</v>
       </c>
       <c r="F262" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G262" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -6764,7 +6760,7 @@
         <v>211</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D263" s="5" t="s">
         <v>5</v>
@@ -6776,7 +6772,7 @@
         <v>10</v>
       </c>
       <c r="G263" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -6787,7 +6783,7 @@
         <v>211</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D264" s="5" t="s">
         <v>5</v>
@@ -6799,7 +6795,7 @@
         <v>10</v>
       </c>
       <c r="G264" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -6810,7 +6806,7 @@
         <v>211</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D265" s="5" t="s">
         <v>5</v>
@@ -6822,60 +6818,52 @@
         <v>10</v>
       </c>
       <c r="G265" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D266" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E266" s="5">
-        <v>0</v>
-      </c>
-      <c r="F266" s="5">
-        <v>10</v>
-      </c>
-      <c r="G266" s="5">
-        <v>0</v>
+        <v>220</v>
+      </c>
+      <c r="D266" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E266" s="7"/>
+      <c r="F266" s="7"/>
+      <c r="G266" s="11" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>211</v>
+        <v>228</v>
+      </c>
+      <c r="B267" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D267" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E267" s="5">
-        <v>0</v>
-      </c>
-      <c r="F267" s="5">
-        <v>10</v>
-      </c>
-      <c r="G267" s="5">
-        <v>0</v>
+        <v>230</v>
+      </c>
+      <c r="D267" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E267" s="7"/>
+      <c r="F267" s="7"/>
+      <c r="G267" s="6" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B268" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B268" s="7" t="s">
         <v>226</v>
       </c>
       <c r="C268" s="4" t="s">
@@ -6884,45 +6872,7 @@
       <c r="D268" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E268" s="7"/>
-      <c r="F268" s="7"/>
-      <c r="G268" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A269" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B269" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C269" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D269" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E269" s="7"/>
-      <c r="F269" s="7"/>
-      <c r="G269" s="6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A270" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B270" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C270" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D270" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G270" t="s">
+      <c r="G268" t="s">
         <v>232</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Lidar rain model
Changed the configuration for the Point Cloud sensor in Prescan:
- kept only the front sensor
- changed from 16 to 32 vertical beams
- changed from 225 to 256 beams per 90 degrees
- changed vertical FoV from 30 to 45 degrees
- changed far clipping distance to 150 m
- changed close clipping distance to 0.25 m

In Simulink:
- changed the library so that it works with the new number of points
- changed z_max to 105m

In the Lidar model:
- changed the reflectivity to come as a gain on the intensity input (it used to be part of the intensity threshold, that one is now fixed at 0.8)
- added a 1/ range ^2 * pi factor to the intensity to simulate the intensity drop (1 / range ^2) and the conversion from reflectivity to back scattering coefficient (1 / pi)

Other modifications:
- created a new xosc file with the subset
- fixed the lidar_euclidean cluster config in the AutowareConfigTemplate
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C9C839-950E-4556-9E8A-F143BEB6E9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745874DA-BAE0-45B9-A8B0-DA705745E792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15996" yWindow="1272" windowWidth="14724" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G149" sqref="G149"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4128,7 +4128,7 @@
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
       <c r="G141" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -4151,7 +4151,7 @@
         <v>1</v>
       </c>
       <c r="G142" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -4296,7 +4296,7 @@
         <v>10</v>
       </c>
       <c r="G149" s="5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -4586,7 +4586,7 @@
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
       <c r="G163" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Increased decceleration is autoware config
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745874DA-BAE0-45B9-A8B0-DA705745E792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B46230-6EAF-498E-9759-8B1B5FAEAB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,21 +1138,21 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G164" sqref="G164"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G223" sqref="G223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="1" customWidth="1"/>
-    <col min="7" max="7" width="134.6640625" customWidth="1"/>
+    <col min="7" max="7" width="134.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>224</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>224</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>224</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>224</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>224</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>224</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>224</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>224</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>224</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>23</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>23</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>23</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>23</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>-0.37059999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>-0.62939999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>23</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>23</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>23</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>23</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>23</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>23</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>23</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>23</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>23</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>23</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>23</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>23</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>23</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>23</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>23</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>23</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>23</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>23</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>23</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>23</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>23</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>23</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>23</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>23</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>23</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>23</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>23</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>23</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>23</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>23</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>23</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>23</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>23</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>23</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>23</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>23</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>23</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>23</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>23</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>23</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>23</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>23</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>23</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>23</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>23</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>23</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>23</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>23</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>23</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>23</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>23</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>23</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>23</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>23</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>23</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>23</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>23</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>23</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>23</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>23</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>23</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>23</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>23</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>23</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>23</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>23</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>23</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>23</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>23</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>23</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>23</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>23</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>23</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>23</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>23</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>23</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>23</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>23</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>23</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>23</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>23</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>23</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>23</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>23</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>23</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>23</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>23</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>23</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>23</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>23</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>23</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>23</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>23</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>23</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>23</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>23</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>23</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>23</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>23</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>23</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>23</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>23</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>23</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>23</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>23</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>23</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>23</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>23</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>23</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>23</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>23</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>23</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>23</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>23</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>23</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>23</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>23</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>23</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>23</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>23</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>23</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>23</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>23</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>23</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>23</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>23</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>23</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>23</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>23</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>213</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>213</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>213</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>213</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>213</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>213</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>213</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>213</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>213</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>214</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>214</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>214</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>214</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>214</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>214</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>214</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>214</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>214</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>214</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>214</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>214</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>214</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>214</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>214</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>214</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>214</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>214</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>214</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>214</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>214</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>214</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>214</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>214</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>214</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>214</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>214</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>214</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>214</v>
       </c>
@@ -5808,10 +5808,10 @@
         <v>10</v>
       </c>
       <c r="G221" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>214</v>
       </c>
@@ -5831,10 +5831,10 @@
         <v>0</v>
       </c>
       <c r="G222" s="5">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>214</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>214</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>214</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>214</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>214</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>214</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>214</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>214</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>214</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>214</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>214</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>214</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>214</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>214</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>226</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>228</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
Disabled ground removal in TA
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B46230-6EAF-498E-9759-8B1B5FAEAB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FDDE17-A06F-42D7-9B26-D0B498AB06C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1138,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G223" sqref="G223"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4109,7 +4109,7 @@
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
       <c r="G140" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Increase lateral distance of local planner
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
+++ b/AD-EYE/TA/Configurations/AutowareConfigTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FDDE17-A06F-42D7-9B26-D0B498AB06C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC759D2F-0F27-453F-8F2E-07CC65D78073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1138,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G214" sqref="G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5460,7 +5460,7 @@
         <v>10</v>
       </c>
       <c r="G205" s="5">
-        <v>0.1</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -5601,7 +5601,7 @@
         <v>10</v>
       </c>
       <c r="G212" s="5">
-        <v>2.2000000000000002</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -5624,7 +5624,7 @@
         <v>10</v>
       </c>
       <c r="G213" s="5">
-        <v>4.8</v>
+        <v>4.79</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>